<commit_message>
updated to algorithm 2026
</commit_message>
<xml_diff>
--- a/Lecturers.xlsx
+++ b/Lecturers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rperezca/Documents/Science/teaching/TD_ABB/TD_ABB copy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rperezca/Documents/Science/teaching/TD_ABB/TD_ABB_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB04DCE7-64A2-454E-A340-17BCDC8FB4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DDA3CA-9AB9-2A43-925C-38EAF8D5695F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="760" windowWidth="28800" windowHeight="17480" xr2:uid="{36AEAC1D-FFDF-4257-B0D1-B6B94AE0B1B2}"/>
+    <workbookView xWindow="720" yWindow="660" windowWidth="28800" windowHeight="17420" xr2:uid="{36AEAC1D-FFDF-4257-B0D1-B6B94AE0B1B2}"/>
   </bookViews>
   <sheets>
     <sheet name="KeywordsANDAffiliation" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="245">
   <si>
     <t>Biophysics</t>
   </si>
@@ -765,6 +765,12 @@
   </si>
   <si>
     <t>email2@ic.ac.uk</t>
+  </si>
+  <si>
+    <t>Overload</t>
+  </si>
+  <si>
+    <t>Tutor</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1351,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1452,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>21</v>
@@ -1484,7 +1490,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -1623,7 +1629,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>243</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>21</v>
@@ -1721,7 +1727,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>21</v>
@@ -1770,7 +1776,7 @@
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>21</v>
@@ -1799,7 +1805,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>21</v>
@@ -1825,7 +1831,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>21</v>
@@ -1857,7 +1863,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>21</v>
@@ -1924,7 +1930,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>21</v>
@@ -2173,7 +2179,7 @@
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>21</v>
@@ -2202,7 +2208,7 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>21</v>
@@ -2254,7 +2260,7 @@
         <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>21</v>
@@ -2283,7 +2289,7 @@
         <v>13</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>21</v>
@@ -2338,7 +2344,7 @@
         <v>8</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>33</v>
+        <v>243</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>21</v>
@@ -2425,7 +2431,7 @@
         <v>8</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>21</v>
@@ -2540,7 +2546,7 @@
         <v>8</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>21</v>
@@ -2569,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>21</v>
@@ -2762,7 +2768,7 @@
         <v>8</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>21</v>
@@ -2846,7 +2852,7 @@
         <v>8</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>21</v>
@@ -2875,7 +2881,7 @@
         <v>11</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>21</v>
@@ -2904,7 +2910,7 @@
         <v>13</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>21</v>
@@ -2933,7 +2939,7 @@
         <v>13</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>21</v>
@@ -2993,7 +2999,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>21</v>
@@ -3042,7 +3048,7 @@
         <v>8</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>21</v>
@@ -3175,7 +3181,7 @@
         <v>12</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>21</v>
@@ -3210,7 +3216,7 @@
         <v>8</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>21</v>
@@ -3242,7 +3248,7 @@
         <v>11</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>21</v>
@@ -3288,7 +3294,7 @@
         <v>8</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>21</v>
@@ -3389,7 +3395,7 @@
         <v>8</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>21</v>
@@ -3530,7 +3536,7 @@
         <v>8</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>21</v>
@@ -3663,7 +3669,7 @@
         <v>13</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G85" s="12" t="s">
         <v>32</v>
@@ -3689,7 +3695,7 @@
         <v>14</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>21</v>
@@ -3747,7 +3753,7 @@
         <v>8</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>21</v>
@@ -3805,7 +3811,7 @@
         <v>8</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>21</v>
@@ -3866,7 +3872,7 @@
         <v>13</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>21</v>
@@ -3944,7 +3950,7 @@
         <v>8</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>21</v>
@@ -4005,7 +4011,7 @@
         <v>14</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>21</v>
@@ -4085,7 +4091,7 @@
         <v>11</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>21</v>
@@ -4140,7 +4146,7 @@
         <v>11</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>21</v>

</xml_diff>